<commit_message>
Latest version of VAR-PBB, as built. Updated under voltage cutout resistor to get UVLO to around 8.1 V.
</commit_message>
<xml_diff>
--- a/VAR-PBB_v01/VAR-PBB_v01_BOM.xlsx
+++ b/VAR-PBB_v01/VAR-PBB_v01_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Engineering-3\VAR-PBB\VAR-PBB_v01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758D1502-5EBC-45CD-B698-936C5613588B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18263703-7AB4-4FA7-B7B5-F19D7A88D6C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -850,9 +850,6 @@
     <t>1M 1% 0603 resistor</t>
   </si>
   <si>
-    <t>220K 1% 0603 resistor</t>
-  </si>
-  <si>
     <t>392 ohm 0603 resistor</t>
   </si>
   <si>
@@ -1057,22 +1054,25 @@
     <t>1 MOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
   </si>
   <si>
-    <t>RMCF0603FT220KCT-ND</t>
-  </si>
-  <si>
-    <t>RMCF0603FT220K</t>
-  </si>
-  <si>
-    <t>220 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
-  </si>
-  <si>
-    <t>RMCF0603FT39R2CT-ND</t>
-  </si>
-  <si>
-    <t>RMCF0603FT39R2</t>
-  </si>
-  <si>
-    <t>39.2 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+    <t>RNCP0603FTD392RCT-ND</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD392R</t>
+  </si>
+  <si>
+    <t>392 Ohms ±1% 0.125W, 1/8W Chip Resistor 0603 (1608 Metric) Anti-Sulfur, Moisture Resistant Thin Film</t>
+  </si>
+  <si>
+    <t>210K 1% 0603 resistor</t>
+  </si>
+  <si>
+    <t>RMCF0603FT210KCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT210K</t>
+  </si>
+  <si>
+    <t>210 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
   </si>
 </sst>
 </file>
@@ -1592,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,7 +1603,7 @@
     <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="7" max="7" width="46.5703125" customWidth="1"/>
+    <col min="7" max="7" width="67.140625" customWidth="1"/>
     <col min="8" max="8" width="47" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1685,7 +1685,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H6" s="24" t="s">
         <v>4</v>
@@ -1709,7 +1709,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H7" s="17" t="s">
         <v>244</v>
@@ -1733,7 +1733,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>245</v>
@@ -1757,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>249</v>
@@ -1781,7 +1781,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H10" s="18" t="s">
         <v>254</v>
@@ -1813,22 +1813,22 @@
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="29" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D12" s="30">
         <v>1327</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F12" s="19">
         <v>1</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1837,66 +1837,66 @@
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="29" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F13" s="19">
         <v>1</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
       <c r="B14" s="17"/>
       <c r="C14" s="29" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F14" s="19">
         <v>2</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="17"/>
       <c r="C15" s="29" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F15" s="19">
         <v>2</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1905,19 +1905,19 @@
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>281</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="E16" s="29" t="s">
         <v>282</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>283</v>
       </c>
       <c r="F16" s="19">
         <v>1</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H16" s="18" t="s">
         <v>260</v>
@@ -1929,19 +1929,19 @@
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>290</v>
-      </c>
       <c r="E17" s="28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F17" s="19">
         <v>1</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H17" s="18" t="s">
         <v>261</v>
@@ -1949,23 +1949,23 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="18" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F18" s="19">
         <v>2</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>262</v>
@@ -1977,19 +1977,19 @@
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="D19" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>330</v>
-      </c>
       <c r="E19" s="28" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F19" s="19">
         <v>1</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H19" s="18" t="s">
         <v>264</v>
@@ -2001,19 +2001,19 @@
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F20" s="19">
         <v>1</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H20" s="27" t="s">
         <v>265</v>
@@ -2025,22 +2025,22 @@
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="F21" s="19">
         <v>1</v>
       </c>
       <c r="G21" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="H21" s="27" t="s">
         <v>337</v>
-      </c>
-      <c r="H21" s="27" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2049,46 +2049,46 @@
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F22" s="19">
         <v>1</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="D23" s="29" t="s">
         <v>278</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="E23" s="29" t="s">
         <v>279</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>280</v>
       </c>
       <c r="F23" s="19">
         <v>7</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -2097,22 +2097,22 @@
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F24" s="19">
         <v>1</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H24" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2121,70 +2121,70 @@
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F25" s="19">
         <v>1</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H25" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="D26" s="18" t="s">
         <v>315</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>316</v>
-      </c>
       <c r="E26" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F26" s="19">
         <v>2</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H26" s="31" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F27" s="19">
         <v>2</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H27" s="31" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>